<commit_message>
feat: Akıl-mantık testi için puzzle stilinde loglama sistemi ve kapsamlı veri analizi raporu
- Puzzle testindeki gibi kolay okunur emoji'li loglama sistemi eklendi
- Her soru, bölüm geçişi ve test sonu için detaylı loglar
- Bölüm bazlı istatistikler (min/max/ortalama tepki süreleri)
- Dürtüsellik analizi (hızlı yanlış cevap tespiti)
- Excel uyumlu 50+ veri noktası tam olarak mevcut
- akil_mantik_veri_analizi.md raporu oluşturuldu
- Console'da gerçek zamanlı veri takibi mümkün
</commit_message>
<xml_diff>
--- a/Rapor/FORTEST-RAPORLAMA-VERİ TABANI-09.07.25-V3.xlsx
+++ b/Rapor/FORTEST-RAPORLAMA-VERİ TABANI-09.07.25-V3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ECE\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Desktop/For Brain/20.07 Bilişsel/Bilişsel Beceri 24-07/Bilişsel Beceriler Testi/Rapor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D04A594-11A9-4E82-BF9C-3E387E44A2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F327BB1A-F254-A441-863B-85A42BE13C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{72AD7830-119C-4DCE-B504-4E14C1F503FB}"/>
+    <workbookView xWindow="-120" yWindow="760" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{72AD7830-119C-4DCE-B504-4E14C1F503FB}"/>
   </bookViews>
   <sheets>
     <sheet name="BECERİ TABLOSU" sheetId="8" r:id="rId1"/>
@@ -33,7 +33,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -830,9 +829,6 @@
     <t xml:space="preserve">9'lu Puzzle Tamamı İçin </t>
   </si>
   <si>
-    <t>Doğru Sayısı / Toplam Parça x 100            (2 parça üzerinden)</t>
-  </si>
-  <si>
     <t>Doğru Sayısı / Toplam Parça x 100            (18 parça üzerinden)</t>
   </si>
   <si>
@@ -897,6 +893,9 @@
   </si>
   <si>
     <t>Bilişsel Esneklik</t>
+  </si>
+  <si>
+    <t>Doğru Sayısı / Toplam Parça x 100            (9 parça üzerinden)</t>
   </si>
 </sst>
 </file>
@@ -907,7 +906,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="162"/>
       <scheme val="minor"/>
@@ -916,13 +915,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="162"/>
       <scheme val="minor"/>
@@ -931,14 +930,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -946,7 +945,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFEE0000"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -954,7 +953,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="162"/>
       <scheme val="minor"/>
@@ -963,7 +962,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1135,7 +1134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1217,14 +1216,34 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1241,38 +1260,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1293,7 +1282,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1303,39 +1292,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1387,7 +1376,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1498,6 +1487,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -1506,13 +1502,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1577,31 +1566,11 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1615,247 +1584,247 @@
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" style="49" customWidth="1"/>
-    <col min="2" max="5" width="9.140625" style="49"/>
-    <col min="6" max="6" width="9.140625" style="49" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="49"/>
+    <col min="1" max="1" width="27.83203125" style="33" customWidth="1"/>
+    <col min="2" max="5" width="9.1640625" style="33"/>
+    <col min="6" max="6" width="9.1640625" style="33" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="C1" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="D1" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="E1" s="32" t="s">
         <v>269</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="F1" s="32" t="s">
         <v>270</v>
       </c>
-      <c r="F1" s="48" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="34" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="B2" s="35" t="s">
         <v>272</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="C2" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
         <v>273</v>
       </c>
-      <c r="C2" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="D2" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="E2" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="F2" s="51" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="B3" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="B3" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="C3" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="D3" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="E3" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="F3" s="51" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="50" t="s">
+      <c r="B4" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="34" t="s">
         <v>275</v>
       </c>
-      <c r="B4" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="C4" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
+      <c r="B5" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="34" t="s">
         <v>276</v>
       </c>
-      <c r="B5" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="C5" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="D5" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="E5" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="F5" s="51" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
+      <c r="B6" s="35"/>
+      <c r="C6" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="34" t="s">
         <v>277</v>
       </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
+      <c r="B7" s="35"/>
+      <c r="C7" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="34" t="s">
         <v>278</v>
       </c>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="50" t="s">
+      <c r="B8" s="35"/>
+      <c r="C8" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="34" t="s">
         <v>279</v>
       </c>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="50" t="s">
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="34" t="s">
         <v>280</v>
       </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="F9" s="51" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="50" t="s">
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="34" t="s">
         <v>281</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="F10" s="51" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="34" t="s">
         <v>282</v>
       </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="F11" s="51" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="50" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="C12" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="D12" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="E12" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="F12" s="51" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="50" t="s">
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="34" t="s">
         <v>283</v>
       </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="E13" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="F13" s="51" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="50" t="s">
-        <v>174</v>
-      </c>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="50" t="s">
-        <v>284</v>
-      </c>
-      <c r="B15" s="51"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1870,19 +1839,19 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="2" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="6" max="6" width="32.1640625" customWidth="1"/>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
     <col min="8" max="8" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
@@ -1893,12 +1862,12 @@
         <v>16</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="32"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F1" s="36"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1921,7 +1890,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1944,7 +1913,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1957,17 +1926,17 @@
       <c r="E4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="37" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1980,11 +1949,11 @@
       <c r="E5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1997,11 +1966,11 @@
       <c r="E6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -2014,11 +1983,11 @@
       <c r="E7" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -2031,11 +2000,11 @@
       <c r="E8" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -2048,11 +2017,11 @@
       <c r="E9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -2073,7 +2042,7 @@
       </c>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -2086,15 +2055,15 @@
       <c r="E11" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="H11" s="31"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="37"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -2107,11 +2076,11 @@
       <c r="E12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -2124,11 +2093,11 @@
       <c r="E13" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -2141,11 +2110,11 @@
       <c r="E14" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>2</v>
@@ -2154,11 +2123,11 @@
       <c r="E15" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -2171,11 +2140,11 @@
       <c r="E16" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -2196,7 +2165,7 @@
       </c>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -2209,15 +2178,15 @@
       <c r="E18" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="G18" s="31" t="s">
+      <c r="G18" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="H18" s="31"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="37"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>17</v>
       </c>
@@ -2230,11 +2199,11 @@
       <c r="E19" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>18</v>
       </c>
@@ -2247,11 +2216,11 @@
       <c r="E20" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>19</v>
       </c>
@@ -2264,11 +2233,11 @@
       <c r="E21" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>20</v>
       </c>
@@ -2281,11 +2250,11 @@
       <c r="E22" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>21</v>
       </c>
@@ -2298,11 +2267,11 @@
       <c r="E23" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>22</v>
       </c>
@@ -2323,7 +2292,7 @@
       </c>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>23</v>
       </c>
@@ -2336,15 +2305,15 @@
       <c r="E25" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F25" s="31" t="s">
+      <c r="F25" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="G25" s="31" t="s">
+      <c r="G25" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="H25" s="31"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="37"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>24</v>
       </c>
@@ -2357,11 +2326,11 @@
       <c r="E26" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>25</v>
       </c>
@@ -2374,11 +2343,11 @@
       <c r="E27" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>26</v>
       </c>
@@ -2391,11 +2360,11 @@
       <c r="E28" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>27</v>
       </c>
@@ -2408,11 +2377,11 @@
       <c r="E29" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>28</v>
       </c>
@@ -2425,11 +2394,11 @@
       <c r="E30" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>29</v>
       </c>
@@ -2443,7 +2412,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>30</v>
       </c>
@@ -2453,19 +2422,19 @@
       <c r="C32" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G32" s="31" t="s">
+      <c r="G32" s="37" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C33" s="3"/>
-      <c r="G33" s="31"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="37"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>31</v>
       </c>
@@ -2475,9 +2444,9 @@
       <c r="C34" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G34" s="31"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="37"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>32</v>
       </c>
@@ -2487,9 +2456,9 @@
       <c r="C35" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="31"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="37"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>33</v>
       </c>
@@ -2499,9 +2468,9 @@
       <c r="C36" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G36" s="31"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="37"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>34</v>
       </c>
@@ -2511,9 +2480,9 @@
       <c r="C37" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G37" s="31"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G37" s="37"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>35</v>
       </c>
@@ -2524,7 +2493,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>36</v>
       </c>
@@ -2535,7 +2504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>37</v>
       </c>
@@ -2546,7 +2515,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>38</v>
       </c>
@@ -2557,7 +2526,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>39</v>
       </c>
@@ -2568,7 +2537,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>40</v>
       </c>
@@ -2579,7 +2548,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>41</v>
       </c>
@@ -2590,7 +2559,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>42</v>
       </c>
@@ -2601,7 +2570,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>43</v>
       </c>
@@ -2612,7 +2581,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>44</v>
       </c>
@@ -2623,7 +2592,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>45</v>
       </c>
@@ -2634,7 +2603,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>46</v>
       </c>
@@ -2645,7 +2614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>47</v>
       </c>
@@ -2656,7 +2625,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>48</v>
       </c>
@@ -2667,7 +2636,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>49</v>
       </c>
@@ -2678,7 +2647,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>50</v>
       </c>
@@ -2691,11 +2660,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="F4:F9"/>
-    <mergeCell ref="F11:F16"/>
-    <mergeCell ref="F18:F23"/>
-    <mergeCell ref="F25:F30"/>
     <mergeCell ref="H4:H9"/>
     <mergeCell ref="H11:H16"/>
     <mergeCell ref="H18:H23"/>
@@ -2705,6 +2669,11 @@
     <mergeCell ref="G11:G16"/>
     <mergeCell ref="G18:G23"/>
     <mergeCell ref="G25:G30"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="F4:F9"/>
+    <mergeCell ref="F11:F16"/>
+    <mergeCell ref="F18:F23"/>
+    <mergeCell ref="F25:F30"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2719,19 +2688,19 @@
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="2" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="6" max="6" width="32.1640625" customWidth="1"/>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
     <col min="8" max="8" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
@@ -2742,14 +2711,14 @@
         <v>97</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -2772,7 +2741,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -2795,7 +2764,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -2808,17 +2777,17 @@
       <c r="E4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="37" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -2831,11 +2800,11 @@
       <c r="E5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -2848,11 +2817,11 @@
       <c r="E6" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>99</v>
@@ -2861,11 +2830,11 @@
       <c r="E7" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -2878,11 +2847,11 @@
       <c r="E8" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -2895,11 +2864,11 @@
       <c r="E9" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -2920,7 +2889,7 @@
       </c>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -2933,17 +2902,17 @@
       <c r="E11" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="37" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -2956,11 +2925,11 @@
       <c r="E12" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
         <v>100</v>
@@ -2969,11 +2938,11 @@
       <c r="E13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>11</v>
       </c>
@@ -2986,11 +2955,11 @@
       <c r="E14" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>12</v>
       </c>
@@ -3003,11 +2972,11 @@
       <c r="E15" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>13</v>
       </c>
@@ -3020,11 +2989,11 @@
       <c r="E16" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>14</v>
       </c>
@@ -3045,7 +3014,7 @@
       </c>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>15</v>
       </c>
@@ -3058,17 +3027,17 @@
       <c r="E18" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="G18" s="31" t="s">
+      <c r="G18" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="H18" s="31" t="s">
+      <c r="H18" s="37" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>101</v>
@@ -3077,11 +3046,11 @@
       <c r="E19" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>16</v>
       </c>
@@ -3094,11 +3063,11 @@
       <c r="E20" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>17</v>
       </c>
@@ -3111,11 +3080,11 @@
       <c r="E21" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>18</v>
       </c>
@@ -3128,11 +3097,11 @@
       <c r="E22" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>19</v>
       </c>
@@ -3145,11 +3114,11 @@
       <c r="E23" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>20</v>
       </c>
@@ -3170,256 +3139,268 @@
       </c>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="28"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
       <c r="E25" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F25" s="31" t="s">
+      <c r="F25" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="G25" s="31" t="s">
+      <c r="G25" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="H25" s="31" t="s">
+      <c r="H25" s="37" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="40"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="40"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="28"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="28"/>
       <c r="E26" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="40"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="40"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="28"/>
       <c r="E27" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="40"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="28"/>
       <c r="E28" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="40"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="40"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="28"/>
       <c r="E29" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="40"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="40"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="28"/>
       <c r="E30" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="40"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="28"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
       <c r="E31" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="F31" s="43" t="s">
+      <c r="F31" s="31" t="s">
         <v>82</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="40"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="40"/>
+    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="28"/>
       <c r="E32" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="F32" s="31" t="s">
+      <c r="F32" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="G32" s="31" t="s">
+      <c r="G32" s="37" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="40"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="40"/>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="28"/>
       <c r="E33" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="40"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="40"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="28"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="28"/>
       <c r="E34" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="40"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="40"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="28"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="28"/>
       <c r="E35" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="40"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="40"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="28"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="28"/>
       <c r="E36" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F36" s="42"/>
-      <c r="G36" s="31"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F36" s="39"/>
+      <c r="G36" s="37"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E37" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F37" s="42"/>
-      <c r="G37" s="31"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F37" s="39"/>
+      <c r="G37" s="37"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E38" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F38" s="44"/>
-      <c r="G38" s="44"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E39" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="F39" s="46"/>
-      <c r="G39" s="46"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E40" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F40" s="46"/>
-      <c r="G40" s="46"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F40" s="40"/>
+      <c r="G40" s="40"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E41" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="F41" s="46"/>
-      <c r="G41" s="46"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F41" s="40"/>
+      <c r="G41" s="40"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E42" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F42" s="46"/>
-      <c r="G42" s="46"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E43" s="44"/>
-      <c r="F43" s="46"/>
-      <c r="G43" s="46"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E44" s="45"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="46"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E45" s="45"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E46" s="45"/>
-      <c r="F46" s="46"/>
-      <c r="G46" s="46"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E47" s="45"/>
-      <c r="F47" s="46"/>
-      <c r="G47" s="46"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E48" s="45"/>
-      <c r="F48" s="46"/>
-      <c r="G48" s="46"/>
-    </row>
-    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E49" s="45"/>
-      <c r="F49" s="46"/>
-      <c r="G49" s="46"/>
-    </row>
-    <row r="50" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E50" s="45"/>
-      <c r="F50" s="46"/>
-      <c r="G50" s="46"/>
-    </row>
-    <row r="51" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E51" s="44"/>
-      <c r="F51" s="46"/>
-      <c r="G51" s="46"/>
-    </row>
-    <row r="52" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E52" s="45"/>
-    </row>
-    <row r="53" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E53" s="45"/>
-    </row>
-    <row r="54" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E54" s="45"/>
-    </row>
-    <row r="55" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E55" s="45"/>
-    </row>
-    <row r="56" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E56" s="45"/>
-    </row>
-    <row r="57" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E57" s="45"/>
-    </row>
-    <row r="58" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E58" s="45"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E43" s="25"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="40"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E44" s="20"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E45" s="20"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E46" s="20"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E47" s="20"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="40"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E48" s="20"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="40"/>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E49" s="20"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="40"/>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E50" s="20"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="40"/>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E51" s="25"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="40"/>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E52" s="20"/>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E53" s="20"/>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E54" s="20"/>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E55" s="20"/>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E56" s="20"/>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E57" s="20"/>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E58" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="F32:F37"/>
+    <mergeCell ref="F39:F44"/>
+    <mergeCell ref="F46:F51"/>
+    <mergeCell ref="G32:G37"/>
+    <mergeCell ref="G39:G44"/>
+    <mergeCell ref="G46:G51"/>
+    <mergeCell ref="F18:F23"/>
+    <mergeCell ref="G18:G23"/>
+    <mergeCell ref="H18:H23"/>
+    <mergeCell ref="F25:F30"/>
+    <mergeCell ref="G25:G30"/>
+    <mergeCell ref="H25:H30"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="F4:F9"/>
     <mergeCell ref="G4:G9"/>
@@ -3427,18 +3408,6 @@
     <mergeCell ref="F11:F16"/>
     <mergeCell ref="G11:G16"/>
     <mergeCell ref="H11:H16"/>
-    <mergeCell ref="F18:F23"/>
-    <mergeCell ref="G18:G23"/>
-    <mergeCell ref="H18:H23"/>
-    <mergeCell ref="F25:F30"/>
-    <mergeCell ref="G25:G30"/>
-    <mergeCell ref="H25:H30"/>
-    <mergeCell ref="F32:F37"/>
-    <mergeCell ref="F39:F44"/>
-    <mergeCell ref="F46:F51"/>
-    <mergeCell ref="G32:G37"/>
-    <mergeCell ref="G39:G44"/>
-    <mergeCell ref="G46:G51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3452,18 +3421,18 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="2" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" customWidth="1"/>
-    <col min="6" max="6" width="58.85546875" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+    <col min="6" max="6" width="58.83203125" customWidth="1"/>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
@@ -3474,30 +3443,30 @@
         <v>140</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="41" t="s">
         <v>258</v>
       </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="11"/>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="35"/>
+      <c r="F2" s="43"/>
       <c r="G2" s="9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -3509,7 +3478,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -3521,11 +3490,11 @@
       <c r="F4" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="44" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -3537,9 +3506,9 @@
       <c r="F5" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="G5" s="37"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G5" s="45"/>
+    </row>
+    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -3551,9 +3520,9 @@
       <c r="F6" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="G6" s="37"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G6" s="45"/>
+    </row>
+    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -3565,9 +3534,9 @@
       <c r="F7" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="G7" s="37"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G7" s="45"/>
+    </row>
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -3579,9 +3548,9 @@
       <c r="F8" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="G8" s="38"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G8" s="46"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -3597,7 +3566,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -3609,11 +3578,11 @@
       <c r="F10" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="44" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -3625,9 +3594,9 @@
       <c r="F11" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="G11" s="37"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G11" s="45"/>
+    </row>
+    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -3639,9 +3608,9 @@
       <c r="F12" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="G12" s="37"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G12" s="45"/>
+    </row>
+    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -3653,9 +3622,9 @@
       <c r="F13" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="G13" s="37"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G13" s="45"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
         <v>138</v>
@@ -3671,7 +3640,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -3683,11 +3652,11 @@
       <c r="F15" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G15" s="44" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -3699,9 +3668,9 @@
       <c r="F16" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="G16" s="37"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="45"/>
+    </row>
+    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -3713,9 +3682,9 @@
       <c r="F17" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="G17" s="37"/>
-    </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="45"/>
+    </row>
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -3727,9 +3696,9 @@
       <c r="F18" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="G18" s="38"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="46"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>17</v>
       </c>
@@ -3745,7 +3714,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>18</v>
       </c>
@@ -3757,11 +3726,11 @@
       <c r="F20" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="G20" s="36" t="s">
+      <c r="G20" s="44" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>19</v>
       </c>
@@ -3773,9 +3742,9 @@
       <c r="F21" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="G21" s="37"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="45"/>
+    </row>
+    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>20</v>
       </c>
@@ -3787,9 +3756,9 @@
       <c r="F22" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="G22" s="37"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="45"/>
+    </row>
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>21</v>
       </c>
@@ -3801,9 +3770,9 @@
       <c r="F23" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="G23" s="38"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="46"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>22</v>
       </c>
@@ -3815,7 +3784,7 @@
       <c r="F24" s="8"/>
       <c r="G24" s="23"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>23</v>
       </c>
@@ -3829,7 +3798,7 @@
       </c>
       <c r="G25" s="24"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>24</v>
       </c>
@@ -3843,7 +3812,7 @@
       </c>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>25</v>
       </c>
@@ -3853,7 +3822,7 @@
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>26</v>
       </c>
@@ -3863,7 +3832,7 @@
       <c r="F28" s="24"/>
       <c r="G28" s="24"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>27</v>
       </c>
@@ -3873,7 +3842,7 @@
       <c r="F29" s="24"/>
       <c r="G29" s="24"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>28</v>
       </c>
@@ -3883,7 +3852,7 @@
       <c r="F30" s="24"/>
       <c r="G30" s="24"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>29</v>
       </c>
@@ -3893,7 +3862,7 @@
       <c r="F31" s="25"/>
       <c r="G31" s="25"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>30</v>
       </c>
@@ -3903,7 +3872,7 @@
       <c r="F32" s="24"/>
       <c r="G32" s="24"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>31</v>
       </c>
@@ -3913,7 +3882,7 @@
       <c r="F33" s="24"/>
       <c r="G33" s="24"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>32</v>
       </c>
@@ -3923,7 +3892,7 @@
       <c r="F34" s="20"/>
       <c r="G34" s="24"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>33</v>
       </c>
@@ -3933,7 +3902,7 @@
       <c r="F35" s="20"/>
       <c r="G35" s="24"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>34</v>
       </c>
@@ -3943,7 +3912,7 @@
       <c r="F36" s="20"/>
       <c r="G36" s="24"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>35</v>
       </c>
@@ -3953,14 +3922,14 @@
       <c r="F37" s="20"/>
       <c r="G37" s="24"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>36</v>
       </c>
@@ -3968,273 +3937,273 @@
       <c r="C39" s="11"/>
       <c r="D39" s="20"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>37</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="11"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>38</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="11"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>39</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="12"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>40</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="12"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>41</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="12"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>42</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="11"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>43</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="12"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>44</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="12"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>45</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="11"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>46</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="12"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>47</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="12"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>48</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="12"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>49</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="11"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>50</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="11"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>51</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="12"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="6">
         <v>52</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="12"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
         <v>53</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="12"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="6">
         <v>54</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="12"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="6">
         <v>55</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="12"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
         <v>56</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="11"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
         <v>57</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="12"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
         <v>58</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="11"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
         <v>59</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="11"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>60</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="12"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
         <v>61</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="11"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
         <v>62</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="12"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="6">
         <v>63</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="11"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="6">
         <v>64</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="12"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="6">
         <v>65</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="11"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="6">
         <v>66</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="11"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
         <v>67</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="11"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="6">
         <v>68</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="12"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
         <v>69</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="12"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="6">
         <v>70</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="12"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="6">
         <v>71</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="12"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="6">
         <v>72</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="11"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="6">
         <v>73</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="12"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="6">
         <v>74</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="11"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="6">
         <v>75</v>
       </c>
@@ -4258,23 +4227,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ABE93D1-6415-48FD-8F5D-5FDD15DF99DD}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView zoomScale="78" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="2" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" customWidth="1"/>
-    <col min="10" max="10" width="61.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="6" max="6" width="32.1640625" customWidth="1"/>
+    <col min="7" max="7" width="32.5" customWidth="1"/>
+    <col min="10" max="10" width="61.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
@@ -4285,12 +4254,12 @@
         <v>205</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="F1" s="32"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F1" s="36"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -4313,7 +4282,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -4336,7 +4305,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -4349,17 +4318,17 @@
       <c r="E4" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="44" t="s">
         <v>246</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="44" t="s">
         <v>188</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -4372,11 +4341,11 @@
       <c r="E5" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -4389,13 +4358,13 @@
       <c r="E6" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
       <c r="J6" s="9" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -4408,13 +4377,13 @@
       <c r="E7" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
       <c r="J7" s="8" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -4437,7 +4406,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -4450,14 +4419,14 @@
       <c r="E9" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="44" t="s">
         <v>252</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="44" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -4470,30 +4439,30 @@
       <c r="E10" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-    </row>
-    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+    </row>
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
       <c r="E11" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="28"/>
       <c r="B12" s="28"/>
       <c r="C12" s="30"/>
       <c r="E12" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="28"/>
       <c r="B13" s="29"/>
       <c r="C13" s="28"/>
@@ -4505,43 +4474,43 @@
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="28"/>
       <c r="B14" s="29"/>
       <c r="C14" s="28"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="36" t="s">
+      <c r="F14" s="44" t="s">
         <v>247</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G14" s="44" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="28"/>
       <c r="B15" s="28"/>
       <c r="C15" s="30"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="28"/>
       <c r="B16" s="29"/>
       <c r="C16" s="28"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="28"/>
       <c r="B17" s="29"/>
       <c r="C17" s="28"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-    </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+    </row>
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="28"/>
       <c r="B18" s="29"/>
       <c r="C18" s="28"/>
@@ -4553,43 +4522,43 @@
         <v>250</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28"/>
       <c r="B19" s="28"/>
       <c r="C19" s="30"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="36" t="s">
-        <v>262</v>
-      </c>
-      <c r="G19" s="36" t="s">
+      <c r="F19" s="44" t="s">
+        <v>284</v>
+      </c>
+      <c r="G19" s="44" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="28"/>
       <c r="B20" s="29"/>
       <c r="C20" s="28"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="28"/>
       <c r="B21" s="29"/>
       <c r="C21" s="28"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="28"/>
       <c r="B22" s="29"/>
       <c r="C22" s="28"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="28"/>
       <c r="B23" s="29"/>
       <c r="C23" s="28"/>
@@ -4601,43 +4570,43 @@
         <v>251</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="28"/>
       <c r="B24" s="29"/>
       <c r="C24" s="28"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="36" t="s">
-        <v>263</v>
-      </c>
-      <c r="G24" s="36" t="s">
+      <c r="F24" s="44" t="s">
+        <v>262</v>
+      </c>
+      <c r="G24" s="44" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="28"/>
       <c r="B25" s="29"/>
       <c r="C25" s="28"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="28"/>
       <c r="B26" s="29"/>
       <c r="C26" s="28"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="28"/>
       <c r="B27" s="29"/>
       <c r="C27" s="28"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="28"/>
       <c r="B28" s="29"/>
       <c r="C28" s="28"/>
@@ -4649,43 +4618,43 @@
         <v>253</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="28"/>
       <c r="B29" s="29"/>
       <c r="C29" s="28"/>
       <c r="E29" s="4"/>
-      <c r="F29" s="36" t="s">
+      <c r="F29" s="44" t="s">
         <v>254</v>
       </c>
-      <c r="G29" s="36" t="s">
+      <c r="G29" s="44" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="28"/>
       <c r="B30" s="29"/>
       <c r="C30" s="28"/>
       <c r="E30" s="4"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="28"/>
       <c r="B31" s="29"/>
       <c r="C31" s="28"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-    </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+    </row>
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="28"/>
       <c r="B32" s="29"/>
       <c r="C32" s="28"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="28"/>
       <c r="B33" s="28"/>
       <c r="C33" s="28"/>
@@ -4696,132 +4665,139 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="28"/>
       <c r="B34" s="29"/>
       <c r="C34" s="28"/>
       <c r="E34" s="25"/>
-      <c r="F34" s="36" t="s">
-        <v>265</v>
+      <c r="F34" s="44" t="s">
+        <v>264</v>
       </c>
       <c r="G34" s="10" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="28"/>
       <c r="B35" s="29"/>
       <c r="C35" s="28"/>
       <c r="E35" s="20"/>
-      <c r="F35" s="37"/>
+      <c r="F35" s="45"/>
       <c r="G35" s="25"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="28"/>
       <c r="B36" s="29"/>
       <c r="C36" s="28"/>
       <c r="E36" s="20"/>
-      <c r="F36" s="37"/>
+      <c r="F36" s="45"/>
       <c r="G36" s="24"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="28"/>
       <c r="B37" s="29"/>
       <c r="C37" s="28"/>
       <c r="E37" s="20"/>
-      <c r="F37" s="38"/>
+      <c r="F37" s="46"/>
       <c r="G37" s="24"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="28"/>
       <c r="B38" s="29"/>
       <c r="C38" s="28"/>
       <c r="E38" s="20"/>
       <c r="G38" s="24"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="28"/>
       <c r="B39" s="29"/>
       <c r="C39" s="28"/>
       <c r="E39" s="20"/>
       <c r="G39" s="24"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="28"/>
       <c r="B40" s="29"/>
       <c r="C40" s="28"/>
       <c r="E40" s="20"/>
       <c r="G40" s="24"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="28"/>
       <c r="B41" s="29"/>
       <c r="C41" s="28"/>
       <c r="E41" s="20"/>
       <c r="G41" s="24"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="28"/>
       <c r="B42" s="29"/>
       <c r="C42" s="28"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="28"/>
       <c r="B43" s="29"/>
       <c r="C43" s="28"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="28"/>
       <c r="B44" s="29"/>
       <c r="C44" s="28"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="28"/>
       <c r="B45" s="29"/>
       <c r="C45" s="28"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="28"/>
       <c r="B46" s="29"/>
       <c r="C46" s="28"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="28"/>
       <c r="B47" s="29"/>
       <c r="C47" s="28"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="28"/>
       <c r="B48" s="29"/>
       <c r="C48" s="28"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="28"/>
       <c r="B49" s="29"/>
       <c r="C49" s="28"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="28"/>
       <c r="B50" s="29"/>
       <c r="C50" s="28"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="28"/>
       <c r="B51" s="29"/>
       <c r="C51" s="28"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="28"/>
       <c r="B52" s="29"/>
       <c r="C52" s="28"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="28"/>
       <c r="B53" s="29"/>
       <c r="C53" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="G29:G32"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="F4:F7"/>
     <mergeCell ref="F9:F12"/>
@@ -4829,13 +4805,6 @@
     <mergeCell ref="G4:G7"/>
     <mergeCell ref="G9:G12"/>
     <mergeCell ref="G14:G17"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="G29:G32"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4846,23 +4815,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F56B6D1-D890-427E-AAEB-370D022B49D9}">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="107" workbookViewId="0">
+    <sheetView zoomScale="76" zoomScaleNormal="107" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="2" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" customWidth="1"/>
-    <col min="8" max="8" width="41.28515625" customWidth="1"/>
+    <col min="2" max="2" width="38.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="6" max="6" width="32.1640625" customWidth="1"/>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
@@ -4873,12 +4842,12 @@
         <v>205</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="F1" s="32"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F1" s="36"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -4899,7 +4868,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -4920,7 +4889,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -4931,17 +4900,17 @@
       <c r="E4" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="44" t="s">
         <v>202</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="37" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -4952,11 +4921,11 @@
       <c r="E5" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="31"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="37"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -4967,11 +4936,11 @@
       <c r="E6" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="37"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -4982,11 +4951,11 @@
       <c r="E7" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="37"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -5003,9 +4972,9 @@
       <c r="G8" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H8" s="31"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" s="37"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -5016,15 +4985,15 @@
       <c r="E9" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="44" t="s">
         <v>203</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="31"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="37"/>
+    </row>
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>227</v>
@@ -5035,11 +5004,11 @@
       <c r="E10" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -5050,13 +5019,13 @@
       <c r="E11" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="31" t="s">
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="37" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -5067,11 +5036,11 @@
       <c r="E12" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="31"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="37"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -5088,9 +5057,9 @@
       <c r="G13" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H13" s="31"/>
-    </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="37"/>
+    </row>
+    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -5101,15 +5070,15 @@
       <c r="E14" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="F14" s="36" t="s">
+      <c r="F14" s="44" t="s">
         <v>204</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G14" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="H14" s="31"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" s="37"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -5120,11 +5089,11 @@
       <c r="E15" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="31"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="37"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -5135,11 +5104,11 @@
       <c r="E16" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="37"/>
+    </row>
+    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
         <v>228</v>
@@ -5150,11 +5119,11 @@
       <c r="E17" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>15</v>
       </c>
@@ -5171,11 +5140,11 @@
       <c r="G18" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="H18" s="31" t="s">
+      <c r="H18" s="37" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>16</v>
       </c>
@@ -5186,15 +5155,15 @@
       <c r="E19" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="F19" s="36" t="s">
+      <c r="F19" s="44" t="s">
         <v>204</v>
       </c>
-      <c r="G19" s="36" t="s">
+      <c r="G19" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="H19" s="31"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="37"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>17</v>
       </c>
@@ -5205,11 +5174,11 @@
       <c r="E20" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="31"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="37"/>
+    </row>
+    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
         <v>229</v>
@@ -5220,11 +5189,11 @@
       <c r="E21" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="31"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="37"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>18</v>
       </c>
@@ -5235,11 +5204,11 @@
       <c r="E22" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="31"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="37"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>19</v>
       </c>
@@ -5256,9 +5225,9 @@
       <c r="G23" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="H23" s="31"/>
-    </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="37"/>
+    </row>
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>20</v>
       </c>
@@ -5269,15 +5238,15 @@
       <c r="E24" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="F24" s="36" t="s">
+      <c r="F24" s="44" t="s">
         <v>204</v>
       </c>
-      <c r="G24" s="36" t="s">
+      <c r="G24" s="44" t="s">
         <v>133</v>
       </c>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
         <v>230</v>
@@ -5288,13 +5257,13 @@
       <c r="E25" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
       <c r="H25" s="47" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>21</v>
       </c>
@@ -5305,11 +5274,11 @@
       <c r="E26" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="31"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="37"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>22</v>
       </c>
@@ -5320,11 +5289,11 @@
       <c r="E27" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="31"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="37"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>23</v>
       </c>
@@ -5341,55 +5310,55 @@
       <c r="G28" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H28" s="31"/>
-    </row>
-    <row r="29" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="37"/>
+    </row>
+    <row r="29" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
       <c r="E29" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="F29" s="36" t="s">
+      <c r="F29" s="44" t="s">
         <v>259</v>
       </c>
-      <c r="G29" s="36" t="s">
+      <c r="G29" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="H29" s="31"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="37"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="5"/>
       <c r="C30" s="6"/>
       <c r="E30" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="31"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="37"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="28"/>
       <c r="B31" s="29"/>
       <c r="C31" s="28"/>
       <c r="E31" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+    </row>
+    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="28"/>
       <c r="B32" s="29"/>
       <c r="C32" s="28"/>
       <c r="E32" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="28"/>
       <c r="B33" s="28"/>
       <c r="C33" s="28"/>
@@ -5397,7 +5366,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="28"/>
       <c r="B34" s="29"/>
       <c r="C34" s="28"/>
@@ -5406,117 +5375,122 @@
         <v>233</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="28"/>
       <c r="B35" s="29"/>
       <c r="C35" s="28"/>
       <c r="E35" s="20"/>
       <c r="G35" s="25"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="28"/>
       <c r="B36" s="29"/>
       <c r="C36" s="28"/>
       <c r="E36" s="20"/>
       <c r="G36" s="24"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="28"/>
       <c r="B37" s="29"/>
       <c r="C37" s="28"/>
       <c r="E37" s="20"/>
       <c r="G37" s="24"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="28"/>
       <c r="B38" s="29"/>
       <c r="C38" s="28"/>
       <c r="E38" s="20"/>
       <c r="G38" s="24"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="28"/>
       <c r="B39" s="29"/>
       <c r="C39" s="28"/>
       <c r="E39" s="20"/>
       <c r="G39" s="24"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="28"/>
       <c r="B40" s="29"/>
       <c r="C40" s="28"/>
       <c r="E40" s="20"/>
       <c r="G40" s="24"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="28"/>
       <c r="B41" s="29"/>
       <c r="C41" s="28"/>
       <c r="E41" s="20"/>
       <c r="G41" s="24"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="28"/>
       <c r="B42" s="29"/>
       <c r="C42" s="28"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="28"/>
       <c r="B43" s="29"/>
       <c r="C43" s="28"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="28"/>
       <c r="B44" s="29"/>
       <c r="C44" s="28"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="28"/>
       <c r="B45" s="29"/>
       <c r="C45" s="28"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="28"/>
       <c r="B46" s="29"/>
       <c r="C46" s="28"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="28"/>
       <c r="B47" s="29"/>
       <c r="C47" s="28"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="28"/>
       <c r="B48" s="29"/>
       <c r="C48" s="28"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="28"/>
       <c r="B49" s="29"/>
       <c r="C49" s="28"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="28"/>
       <c r="B50" s="29"/>
       <c r="C50" s="28"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="28"/>
       <c r="B51" s="29"/>
       <c r="C51" s="28"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="28"/>
       <c r="B52" s="29"/>
       <c r="C52" s="28"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="28"/>
       <c r="B53" s="29"/>
       <c r="C53" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="G9:G12"/>
     <mergeCell ref="H4:H9"/>
     <mergeCell ref="H11:H16"/>
     <mergeCell ref="H18:H23"/>
@@ -5529,11 +5503,6 @@
     <mergeCell ref="G29:G32"/>
     <mergeCell ref="F14:F17"/>
     <mergeCell ref="G14:G17"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="G4:G7"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="G9:G12"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>